<commit_message>
Se actualiza el cronograma con las actividades realizadas durante la semana
</commit_message>
<xml_diff>
--- a/Cronograma_ProyectoFinal_ ED3.xlsx
+++ b/Cronograma_ProyectoFinal_ ED3.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28318"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Universidad\ED3\Proyecto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69A673EA-EEBB-474A-8216-680D470171C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7C3CCD6-AD46-40EE-9F8E-B1A46BF1602C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E9BA1788-B076-45FF-A5F2-53DAF93C0692}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+  <si>
+    <t xml:space="preserve"># </t>
+  </si>
   <si>
     <t>Tarea</t>
   </si>
@@ -50,12 +53,15 @@
     <t>Recursos</t>
   </si>
   <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>14/10-20/10</t>
+  </si>
+  <si>
     <t>21/10-27/10</t>
   </si>
   <si>
-    <t>14/10-20/10</t>
-  </si>
-  <si>
     <t>28/10 - 03/11</t>
   </si>
   <si>
@@ -89,16 +95,13 @@
     <t>Angee Ocampo</t>
   </si>
   <si>
-    <t xml:space="preserve"># </t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1</t>
   </si>
   <si>
     <t>Presupuesto destinado para el proyecto</t>
   </si>
   <si>
-    <t>Porcentaje</t>
+    <t>Acondicionamiento/Ensamblaje del robot (HW)</t>
   </si>
   <si>
     <t>Angee Ocampo  y José Rivera</t>
@@ -113,61 +116,58 @@
     <t>Implementar el desplazamiento del robot (SW)</t>
   </si>
   <si>
+    <t xml:space="preserve">José Rivera </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>MCU, IDE  y SDK</t>
+  </si>
+  <si>
     <t>Reconocimiento de posición relativa (SW)</t>
   </si>
   <si>
-    <t>Acondicionamiento/Ensamblaje del robot (HW)</t>
+    <t xml:space="preserve">MCU, IDE , SDK, </t>
   </si>
   <si>
     <t>Desarrollo de la interfaz de usuario (SW)</t>
   </si>
   <si>
+    <t>José Rivera</t>
+  </si>
+  <si>
+    <t>MCU, IDE , SDK y pantalla OLED</t>
+  </si>
+  <si>
     <t>Identificación de obstáculos(SW)</t>
   </si>
   <si>
+    <t>MCU, IDE, SDK, y sensor HC-SR04</t>
+  </si>
+  <si>
     <t>Verificación de nivel de batería (SW)</t>
   </si>
   <si>
     <t xml:space="preserve">Etapa de pruebas, validación y corrección </t>
   </si>
   <si>
+    <t>3-8</t>
+  </si>
+  <si>
+    <t>Espacio de prueba</t>
+  </si>
+  <si>
     <t>Diseño e implementación de la carcasa del robot</t>
   </si>
   <si>
-    <t xml:space="preserve">José Rivera </t>
-  </si>
-  <si>
-    <t>José Rivera</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>3-8</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
-    <t>MCU, IDE  y SDK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCU, IDE , SDK, </t>
-  </si>
-  <si>
-    <t>MCU, IDE , SDK y pantalla OLED</t>
-  </si>
-  <si>
-    <t>MCU, IDE, SDK, y sensor HC-SR04</t>
-  </si>
-  <si>
-    <t>Espacio de prueba</t>
+    <t>Convención de colores</t>
   </si>
   <si>
     <t>Completado</t>
-  </si>
-  <si>
-    <t>Convención de colores</t>
   </si>
   <si>
     <t>En proceso</t>
@@ -183,7 +183,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,8 +210,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -248,6 +262,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -276,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -323,7 +343,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -339,9 +359,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -354,6 +371,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,9 +384,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1AD43D"/>
       <color rgb="FFFF7979"/>
       <color rgb="FFF38B35"/>
-      <color rgb="FF1AD43D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -695,81 +717,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A26EDDF-1F76-49D3-A8A6-AC6665F91006}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C15:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15:I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="2"/>
-    <col min="2" max="2" width="47.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" style="2"/>
+    <col min="2" max="2" width="47.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="26" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="E1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="30" t="s">
+      <c r="G1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="H1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="I1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="K1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M1" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="30" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" s="12">
         <v>1</v>
@@ -783,77 +805,77 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="43.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F3" s="15">
         <v>0.8</v>
       </c>
       <c r="G3" s="9"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
       <c r="J3" s="16"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="28.9">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="16"/>
+      <c r="I4" s="13"/>
       <c r="J4" s="16"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F5" s="8">
         <v>0</v>
@@ -861,58 +883,58 @@
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="17"/>
+      <c r="J5" s="31"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F6" s="8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="17"/>
+      <c r="J6" s="31"/>
       <c r="K6" s="17"/>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="28.9">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="E7" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
@@ -923,21 +945,21 @@
       <c r="M7" s="17"/>
       <c r="N7" s="9"/>
     </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="43.15">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F8" s="8">
         <v>0</v>
@@ -951,21 +973,21 @@
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F9" s="8">
         <v>0</v>
@@ -979,21 +1001,21 @@
       <c r="M9" s="18"/>
       <c r="N9" s="9"/>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="28.9">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F10" s="8">
         <v>0</v>
@@ -1007,21 +1029,21 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
     </row>
-    <row r="11" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="28.9">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -1035,35 +1057,191 @@
       <c r="M11" s="9"/>
       <c r="N11" s="19"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="21"/>
+    <row r="13" spans="1:14">
+      <c r="A13" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="30"/>
       <c r="C13" s="20"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15">
       <c r="A14" s="22"/>
       <c r="B14" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="43.5">
       <c r="A15" s="23"/>
       <c r="B15" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="F15" s="5">
+        <v>1</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12">
+        <f>F2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15">
       <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="F16" s="5">
+        <v>2</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" ref="I16:I24" si="0">F3</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="43.5">
       <c r="A17" s="25"/>
       <c r="B17" s="5" t="s">
         <v>46</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15">
+      <c r="F18" s="5">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15">
+      <c r="F19" s="5">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15">
+      <c r="F20" s="5">
+        <v>6</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15">
+      <c r="F21" s="5">
+        <v>7</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15">
+      <c r="F22" s="5">
+        <v>8</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="43.5">
+      <c r="F23" s="5">
+        <v>9</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="43.5">
+      <c r="F24" s="5">
+        <v>10</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>